<commit_message>
EPBDS-9041 fix Comparison_ne tests for primitives
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_ne-alt.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_ne-alt.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\.openl-webstudio\user-workspace\admin\EPBDS-9041_11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99533086-9C17-44D0-9BA1-F7F9B3281B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="6276" yWindow="4896" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NE_ALT" sheetId="22" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1825,7 +1839,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1849,7 +1863,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1859,6 +1873,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1907,7 +1927,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1930,11 +1950,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="ACT_H" xfId="2"/>
+    <cellStyle name="ACT_H" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1992,7 +2013,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2025,9 +2046,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2060,6 +2098,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2235,41 +2290,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:AE381"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K121" sqref="K121:Z121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="2.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="18.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="18.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="2.88671875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="17.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="18.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.5546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="18.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="20" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="19.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="19.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.88671875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="20" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="21.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="31" width="9.140625" style="1"/>
-    <col min="32" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="25" max="25" width="20.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="21.44140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="31" width="9.109375" style="1"/>
+    <col min="32" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="11" t="s">
         <v>578</v>
       </c>
@@ -2297,7 +2352,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
         <v>0</v>
@@ -2369,7 +2424,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
@@ -2443,7 +2498,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>601</v>
       </c>
@@ -2543,7 +2598,7 @@
         <v>= $X$b1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2639,7 +2694,7 @@
         <v>= $X$s1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2735,7 +2790,7 @@
         <v>= $X$i1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2831,7 +2886,7 @@
         <v>= $X$l1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2927,7 +2982,7 @@
         <v>= $X$f1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>36</v>
       </c>
@@ -3023,7 +3078,7 @@
         <v>= $X$d1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="C12" s="1" t="s">
         <v>37</v>
@@ -3120,7 +3175,7 @@
         <v>= $X$B1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
@@ -3216,7 +3271,7 @@
         <v>= $X$S1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
@@ -3312,7 +3367,7 @@
         <v>= $X$I1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
@@ -3408,7 +3463,7 @@
         <v>= $X$L1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
         <v>41</v>
       </c>
@@ -3504,7 +3559,7 @@
         <v>= $X$F1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
@@ -3600,7 +3655,7 @@
         <v>= $X$D1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>43</v>
       </c>
@@ -3696,7 +3751,7 @@
         <v>= $X$BI1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>44</v>
       </c>
@@ -3792,7 +3847,7 @@
         <v>= $X$BD1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
@@ -3888,7 +3943,7 @@
         <v>= $X$BV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
@@ -3984,7 +4039,7 @@
         <v>= $X$SV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
@@ -4080,7 +4135,7 @@
         <v>= $X$IV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
@@ -4176,7 +4231,7 @@
         <v>= $X$LV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
@@ -4272,7 +4327,7 @@
         <v>= $X$FV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>50</v>
       </c>
@@ -4368,7 +4423,7 @@
         <v>= $X$DV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
@@ -4464,7 +4519,7 @@
         <v>= $X$BIV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>52</v>
       </c>
@@ -4560,7 +4615,7 @@
         <v>= $X$BDV1 &lt;&gt; $BDV2$Y</v>
       </c>
     </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C33" s="10" t="s">
         <v>579</v>
       </c>
@@ -4590,7 +4645,7 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
         <v>53</v>
       </c>
@@ -4664,7 +4719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>55</v>
       </c>
@@ -4738,7 +4793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C36" s="7">
         <v>1</v>
       </c>
@@ -4812,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C37" s="7">
         <v>-1</v>
       </c>
@@ -4886,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C38" s="6">
         <v>0</v>
       </c>
@@ -4960,7 +5015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C39" s="6">
         <v>-15</v>
       </c>
@@ -5034,7 +5089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C40" s="6">
         <v>-15</v>
       </c>
@@ -5108,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
       <c r="D41" s="8"/>
       <c r="E41" s="6" t="b">
@@ -5129,56 +5184,56 @@
       <c r="J41" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C42" s="6">
         <v>15</v>
       </c>
@@ -5250,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
       <c r="D43" s="8">
         <v>15</v>
@@ -5322,7 +5377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C44" s="6">
         <v>15</v>
       </c>
@@ -5396,7 +5451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C45" s="6">
         <v>-3</v>
       </c>
@@ -5470,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C49" s="10" t="s">
         <v>580</v>
       </c>
@@ -5500,7 +5555,7 @@
       <c r="Y49" s="6"/>
       <c r="Z49" s="6"/>
     </row>
-    <row r="50" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C50" s="6" t="s">
         <v>53</v>
       </c>
@@ -5574,7 +5629,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
         <v>55</v>
       </c>
@@ -5648,7 +5703,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C52" s="7">
         <v>1</v>
       </c>
@@ -5722,7 +5777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C53" s="7">
         <v>-1</v>
       </c>
@@ -5796,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C54" s="6">
         <v>0</v>
       </c>
@@ -5870,7 +5925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C55" s="6">
         <v>-15</v>
       </c>
@@ -5944,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C56" s="6">
         <v>-15</v>
       </c>
@@ -6018,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C57" s="6"/>
       <c r="D57" s="8"/>
       <c r="E57" s="6" t="b">
@@ -6039,56 +6094,56 @@
       <c r="J57" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C58" s="6">
         <v>15</v>
       </c>
@@ -6160,7 +6215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C59" s="6"/>
       <c r="D59" s="8">
         <v>15</v>
@@ -6232,7 +6287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C60" s="6">
         <v>15</v>
       </c>
@@ -6306,7 +6361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C61" s="6">
         <v>-3</v>
       </c>
@@ -6380,7 +6435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C65" s="10" t="s">
         <v>581</v>
       </c>
@@ -6410,7 +6465,7 @@
       <c r="Y65" s="6"/>
       <c r="Z65" s="6"/>
     </row>
-    <row r="66" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C66" s="6" t="s">
         <v>53</v>
       </c>
@@ -6484,7 +6539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="67" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C67" s="6" t="s">
         <v>55</v>
       </c>
@@ -6558,7 +6613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C68" s="7">
         <v>1</v>
       </c>
@@ -6632,7 +6687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C69" s="7">
         <v>-1</v>
       </c>
@@ -6706,7 +6761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C70" s="6">
         <v>0</v>
       </c>
@@ -6780,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C71" s="6">
         <v>-15</v>
       </c>
@@ -6854,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C72" s="6">
         <v>-15</v>
       </c>
@@ -6928,7 +6983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C73" s="6"/>
       <c r="D73" s="8"/>
       <c r="E73" s="6" t="b">
@@ -6949,56 +7004,56 @@
       <c r="J73" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y73" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z73" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y73" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z73" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C74" s="6">
         <v>15</v>
       </c>
@@ -7070,7 +7125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C75" s="6"/>
       <c r="D75" s="8">
         <v>15</v>
@@ -7142,7 +7197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C76" s="6">
         <v>15</v>
       </c>
@@ -7216,7 +7271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C77" s="6">
         <v>-3</v>
       </c>
@@ -7290,7 +7345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C81" s="10" t="s">
         <v>582</v>
       </c>
@@ -7320,7 +7375,7 @@
       <c r="Y81" s="6"/>
       <c r="Z81" s="6"/>
     </row>
-    <row r="82" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C82" s="6" t="s">
         <v>53</v>
       </c>
@@ -7394,7 +7449,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="83" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C83" s="6" t="s">
         <v>55</v>
       </c>
@@ -7468,7 +7523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C84" s="7">
         <v>1</v>
       </c>
@@ -7542,7 +7597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C85" s="7">
         <v>-1</v>
       </c>
@@ -7616,7 +7671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C86" s="6">
         <v>0</v>
       </c>
@@ -7690,7 +7745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C87" s="6">
         <v>-15</v>
       </c>
@@ -7764,7 +7819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C88" s="6">
         <v>-15</v>
       </c>
@@ -7838,7 +7893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C89" s="6"/>
       <c r="D89" s="8"/>
       <c r="E89" s="6" t="b">
@@ -7859,56 +7914,56 @@
       <c r="J89" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y89" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z89" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y89" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z89" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C90" s="6">
         <v>15</v>
       </c>
@@ -7980,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C91" s="6"/>
       <c r="D91" s="8">
         <v>15</v>
@@ -8052,7 +8107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C92" s="6">
         <v>15</v>
       </c>
@@ -8126,7 +8181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C93" s="6">
         <v>-3</v>
       </c>
@@ -8200,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C97" s="10" t="s">
         <v>583</v>
       </c>
@@ -8230,7 +8285,7 @@
       <c r="Y97" s="6"/>
       <c r="Z97" s="6"/>
     </row>
-    <row r="98" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C98" s="6" t="s">
         <v>53</v>
       </c>
@@ -8304,7 +8359,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C99" s="6" t="s">
         <v>55</v>
       </c>
@@ -8378,7 +8433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C100" s="7">
         <v>1</v>
       </c>
@@ -8452,7 +8507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C101" s="7">
         <v>-1</v>
       </c>
@@ -8526,7 +8581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C102" s="6">
         <v>0</v>
       </c>
@@ -8600,7 +8655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C103" s="6">
         <v>-15</v>
       </c>
@@ -8674,7 +8729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C104" s="6">
         <v>-15</v>
       </c>
@@ -8748,7 +8803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C105" s="6"/>
       <c r="D105" s="8"/>
       <c r="E105" s="6" t="b">
@@ -8769,56 +8824,56 @@
       <c r="J105" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y105" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z105" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y105" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z105" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C106" s="6">
         <v>15</v>
       </c>
@@ -8890,7 +8945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C107" s="6"/>
       <c r="D107" s="8">
         <v>15</v>
@@ -8962,7 +9017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C108" s="6">
         <v>15</v>
       </c>
@@ -9036,7 +9091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C109" s="6">
         <v>-3</v>
       </c>
@@ -9110,7 +9165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C113" s="10" t="s">
         <v>584</v>
       </c>
@@ -9140,7 +9195,7 @@
       <c r="Y113" s="6"/>
       <c r="Z113" s="6"/>
     </row>
-    <row r="114" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C114" s="6" t="s">
         <v>53</v>
       </c>
@@ -9214,7 +9269,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C115" s="6" t="s">
         <v>55</v>
       </c>
@@ -9288,7 +9343,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="116" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C116" s="7">
         <v>1</v>
       </c>
@@ -9362,7 +9417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C117" s="7">
         <v>-1</v>
       </c>
@@ -9436,7 +9491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C118" s="6">
         <v>0</v>
       </c>
@@ -9510,7 +9565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C119" s="6">
         <v>-15</v>
       </c>
@@ -9584,7 +9639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C120" s="6">
         <v>-15</v>
       </c>
@@ -9658,7 +9713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C121" s="6"/>
       <c r="D121" s="8"/>
       <c r="E121" s="6" t="b">
@@ -9679,56 +9734,56 @@
       <c r="J121" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="K121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="M121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="N121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="O121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="P121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="R121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="U121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="V121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="W121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="X121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y121" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z121" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="3:26" x14ac:dyDescent="0.2">
+      <c r="K121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="V121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="X121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y121" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z121" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C122" s="6">
         <v>15</v>
       </c>
@@ -9800,7 +9855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C123" s="6"/>
       <c r="D123" s="8">
         <v>15</v>
@@ -9872,7 +9927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C124" s="6">
         <v>15</v>
       </c>
@@ -9946,7 +10001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C125" s="6">
         <v>-3</v>
       </c>
@@ -10020,7 +10075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C129" s="10" t="s">
         <v>585</v>
       </c>
@@ -10050,7 +10105,7 @@
       <c r="Y129" s="6"/>
       <c r="Z129" s="6"/>
     </row>
-    <row r="130" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C130" s="6" t="s">
         <v>53</v>
       </c>
@@ -10124,7 +10179,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="131" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C131" s="6" t="s">
         <v>55</v>
       </c>
@@ -10198,7 +10253,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C132" s="7">
         <v>1</v>
       </c>
@@ -10272,7 +10327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C133" s="7">
         <v>-1</v>
       </c>
@@ -10346,7 +10401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C134" s="6">
         <v>0</v>
       </c>
@@ -10420,7 +10475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C135" s="6">
         <v>-15</v>
       </c>
@@ -10494,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C136" s="6">
         <v>-15</v>
       </c>
@@ -10568,26 +10623,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C137" s="6"/>
       <c r="D137" s="8"/>
-      <c r="E137" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F137" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G137" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H137" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I137" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J137" s="6" t="b">
-        <v>0</v>
+      <c r="E137" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F137" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G137" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H137" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I137" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J137" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K137" s="6" t="b">
         <v>0</v>
@@ -10638,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C138" s="6">
         <v>15</v>
       </c>
@@ -10710,7 +10765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C139" s="6"/>
       <c r="D139" s="8">
         <v>15</v>
@@ -10782,7 +10837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C140" s="6">
         <v>15</v>
       </c>
@@ -10856,7 +10911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C141" s="6">
         <v>-3</v>
       </c>
@@ -10930,7 +10985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C145" s="10" t="s">
         <v>586</v>
       </c>
@@ -10960,7 +11015,7 @@
       <c r="Y145" s="6"/>
       <c r="Z145" s="6"/>
     </row>
-    <row r="146" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C146" s="6" t="s">
         <v>53</v>
       </c>
@@ -11034,7 +11089,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="147" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C147" s="6" t="s">
         <v>55</v>
       </c>
@@ -11108,7 +11163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C148" s="7">
         <v>1</v>
       </c>
@@ -11182,7 +11237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C149" s="7">
         <v>-1</v>
       </c>
@@ -11256,7 +11311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C150" s="6">
         <v>0</v>
       </c>
@@ -11330,7 +11385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C151" s="6">
         <v>-15</v>
       </c>
@@ -11404,7 +11459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C152" s="6">
         <v>-15</v>
       </c>
@@ -11478,26 +11533,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C153" s="6"/>
       <c r="D153" s="8"/>
-      <c r="E153" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F153" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G153" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H153" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I153" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J153" s="6" t="b">
-        <v>0</v>
+      <c r="E153" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G153" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H153" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I153" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J153" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K153" s="6" t="b">
         <v>0</v>
@@ -11548,7 +11603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C154" s="6">
         <v>15</v>
       </c>
@@ -11620,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C155" s="6"/>
       <c r="D155" s="8">
         <v>15</v>
@@ -11692,7 +11747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C156" s="6">
         <v>15</v>
       </c>
@@ -11766,7 +11821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C157" s="6">
         <v>-3</v>
       </c>
@@ -11840,7 +11895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C161" s="10" t="s">
         <v>587</v>
       </c>
@@ -11870,7 +11925,7 @@
       <c r="Y161" s="6"/>
       <c r="Z161" s="6"/>
     </row>
-    <row r="162" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C162" s="6" t="s">
         <v>53</v>
       </c>
@@ -11944,7 +11999,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="163" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C163" s="6" t="s">
         <v>55</v>
       </c>
@@ -12018,7 +12073,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C164" s="7">
         <v>1</v>
       </c>
@@ -12092,7 +12147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C165" s="7">
         <v>-1</v>
       </c>
@@ -12166,7 +12221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C166" s="6">
         <v>0</v>
       </c>
@@ -12240,7 +12295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C167" s="6">
         <v>-15</v>
       </c>
@@ -12314,7 +12369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C168" s="6">
         <v>-15</v>
       </c>
@@ -12388,26 +12443,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C169" s="6"/>
       <c r="D169" s="8"/>
-      <c r="E169" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F169" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G169" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H169" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I169" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J169" s="6" t="b">
-        <v>0</v>
+      <c r="E169" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F169" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G169" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H169" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I169" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J169" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K169" s="6" t="b">
         <v>0</v>
@@ -12458,7 +12513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C170" s="6">
         <v>15</v>
       </c>
@@ -12530,7 +12585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C171" s="6"/>
       <c r="D171" s="8">
         <v>15</v>
@@ -12602,7 +12657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C172" s="6">
         <v>15</v>
       </c>
@@ -12676,7 +12731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C173" s="6">
         <v>-3</v>
       </c>
@@ -12750,7 +12805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C177" s="10" t="s">
         <v>588</v>
       </c>
@@ -12780,7 +12835,7 @@
       <c r="Y177" s="6"/>
       <c r="Z177" s="6"/>
     </row>
-    <row r="178" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C178" s="6" t="s">
         <v>53</v>
       </c>
@@ -12854,7 +12909,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="179" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C179" s="6" t="s">
         <v>55</v>
       </c>
@@ -12928,7 +12983,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C180" s="7">
         <v>1</v>
       </c>
@@ -13002,7 +13057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C181" s="7">
         <v>-1</v>
       </c>
@@ -13076,7 +13131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C182" s="6">
         <v>0</v>
       </c>
@@ -13150,7 +13205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C183" s="6">
         <v>-15</v>
       </c>
@@ -13224,7 +13279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C184" s="6">
         <v>-15</v>
       </c>
@@ -13298,26 +13353,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C185" s="6"/>
       <c r="D185" s="8"/>
-      <c r="E185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I185" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J185" s="6" t="b">
-        <v>0</v>
+      <c r="E185" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F185" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G185" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H185" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I185" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J185" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K185" s="6" t="b">
         <v>0</v>
@@ -13368,7 +13423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C186" s="6">
         <v>15</v>
       </c>
@@ -13440,7 +13495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C187" s="6"/>
       <c r="D187" s="8">
         <v>15</v>
@@ -13512,7 +13567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C188" s="6">
         <v>15</v>
       </c>
@@ -13586,7 +13641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C189" s="6">
         <v>-3</v>
       </c>
@@ -13660,7 +13715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C193" s="10" t="s">
         <v>589</v>
       </c>
@@ -13690,7 +13745,7 @@
       <c r="Y193" s="6"/>
       <c r="Z193" s="6"/>
     </row>
-    <row r="194" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C194" s="6" t="s">
         <v>53</v>
       </c>
@@ -13764,7 +13819,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="195" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C195" s="6" t="s">
         <v>55</v>
       </c>
@@ -13838,7 +13893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C196" s="7">
         <v>1</v>
       </c>
@@ -13912,7 +13967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C197" s="7">
         <v>-1</v>
       </c>
@@ -13986,7 +14041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C198" s="6">
         <v>0</v>
       </c>
@@ -14060,7 +14115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C199" s="6">
         <v>-15</v>
       </c>
@@ -14134,7 +14189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C200" s="6">
         <v>-15</v>
       </c>
@@ -14208,26 +14263,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C201" s="6"/>
       <c r="D201" s="8"/>
-      <c r="E201" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F201" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G201" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H201" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I201" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J201" s="6" t="b">
-        <v>0</v>
+      <c r="E201" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F201" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G201" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H201" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I201" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J201" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K201" s="6" t="b">
         <v>0</v>
@@ -14278,7 +14333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C202" s="6">
         <v>15</v>
       </c>
@@ -14350,7 +14405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C203" s="6"/>
       <c r="D203" s="8">
         <v>15</v>
@@ -14422,7 +14477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C204" s="6">
         <v>15</v>
       </c>
@@ -14496,7 +14551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C205" s="6">
         <v>-3</v>
       </c>
@@ -14570,7 +14625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C209" s="10" t="s">
         <v>590</v>
       </c>
@@ -14600,7 +14655,7 @@
       <c r="Y209" s="6"/>
       <c r="Z209" s="6"/>
     </row>
-    <row r="210" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C210" s="6" t="s">
         <v>53</v>
       </c>
@@ -14674,7 +14729,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="211" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C211" s="6" t="s">
         <v>55</v>
       </c>
@@ -14748,7 +14803,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="212" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C212" s="7">
         <v>1</v>
       </c>
@@ -14822,7 +14877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C213" s="7">
         <v>-1</v>
       </c>
@@ -14896,7 +14951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C214" s="6">
         <v>0</v>
       </c>
@@ -14970,7 +15025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C215" s="6">
         <v>-15</v>
       </c>
@@ -15044,7 +15099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C216" s="6">
         <v>-15</v>
       </c>
@@ -15118,26 +15173,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C217" s="6"/>
       <c r="D217" s="8"/>
-      <c r="E217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I217" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J217" s="6" t="b">
-        <v>0</v>
+      <c r="E217" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F217" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G217" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H217" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I217" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J217" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K217" s="6" t="b">
         <v>0</v>
@@ -15188,7 +15243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C218" s="6">
         <v>15</v>
       </c>
@@ -15260,7 +15315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C219" s="6"/>
       <c r="D219" s="8">
         <v>15</v>
@@ -15332,7 +15387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C220" s="6">
         <v>15</v>
       </c>
@@ -15406,7 +15461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C221" s="6">
         <v>-3</v>
       </c>
@@ -15480,7 +15535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C225" s="10" t="s">
         <v>591</v>
       </c>
@@ -15510,7 +15565,7 @@
       <c r="Y225" s="6"/>
       <c r="Z225" s="6"/>
     </row>
-    <row r="226" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C226" s="6" t="s">
         <v>53</v>
       </c>
@@ -15584,7 +15639,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="227" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C227" s="6" t="s">
         <v>55</v>
       </c>
@@ -15658,7 +15713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C228" s="7">
         <v>1</v>
       </c>
@@ -15732,7 +15787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C229" s="7">
         <v>-1</v>
       </c>
@@ -15806,7 +15861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C230" s="6">
         <v>0</v>
       </c>
@@ -15880,7 +15935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C231" s="6">
         <v>-15</v>
       </c>
@@ -15954,7 +16009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C232" s="6">
         <v>-15</v>
       </c>
@@ -16028,26 +16083,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C233" s="6"/>
       <c r="D233" s="8"/>
-      <c r="E233" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F233" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G233" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H233" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I233" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J233" s="6" t="b">
-        <v>0</v>
+      <c r="E233" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F233" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G233" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H233" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I233" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J233" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K233" s="6" t="b">
         <v>0</v>
@@ -16098,7 +16153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C234" s="6">
         <v>15</v>
       </c>
@@ -16170,7 +16225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C235" s="6"/>
       <c r="D235" s="8">
         <v>15</v>
@@ -16242,7 +16297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C236" s="6">
         <v>15</v>
       </c>
@@ -16316,7 +16371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C237" s="6">
         <v>-3</v>
       </c>
@@ -16390,7 +16445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="241" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C241" s="10" t="s">
         <v>592</v>
       </c>
@@ -16420,7 +16475,7 @@
       <c r="Y241" s="6"/>
       <c r="Z241" s="6"/>
     </row>
-    <row r="242" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="242" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C242" s="6" t="s">
         <v>53</v>
       </c>
@@ -16494,7 +16549,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="243" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="243" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C243" s="6" t="s">
         <v>55</v>
       </c>
@@ -16568,7 +16623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="244" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C244" s="7">
         <v>1</v>
       </c>
@@ -16642,7 +16697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="245" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C245" s="7">
         <v>-1</v>
       </c>
@@ -16716,7 +16771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="246" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C246" s="6">
         <v>0</v>
       </c>
@@ -16790,7 +16845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="247" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C247" s="6">
         <v>-15</v>
       </c>
@@ -16864,7 +16919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="248" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C248" s="6">
         <v>-15</v>
       </c>
@@ -16938,26 +16993,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="249" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C249" s="6"/>
       <c r="D249" s="8"/>
-      <c r="E249" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F249" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G249" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H249" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I249" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J249" s="6" t="b">
-        <v>0</v>
+      <c r="E249" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F249" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G249" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H249" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I249" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J249" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K249" s="6" t="b">
         <v>0</v>
@@ -17008,7 +17063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="250" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C250" s="6">
         <v>15</v>
       </c>
@@ -17080,7 +17135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="251" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C251" s="6"/>
       <c r="D251" s="8">
         <v>15</v>
@@ -17152,7 +17207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="252" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C252" s="6">
         <v>15</v>
       </c>
@@ -17226,7 +17281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="253" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C253" s="6">
         <v>-3</v>
       </c>
@@ -17300,7 +17355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="257" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C257" s="10" t="s">
         <v>593</v>
       </c>
@@ -17330,7 +17385,7 @@
       <c r="Y257" s="6"/>
       <c r="Z257" s="6"/>
     </row>
-    <row r="258" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="258" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C258" s="6" t="s">
         <v>53</v>
       </c>
@@ -17404,7 +17459,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="259" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="259" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C259" s="6" t="s">
         <v>55</v>
       </c>
@@ -17478,7 +17533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="260" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="260" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C260" s="7">
         <v>1</v>
       </c>
@@ -17552,7 +17607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="261" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C261" s="7">
         <v>-1</v>
       </c>
@@ -17626,7 +17681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="262" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C262" s="6">
         <v>0</v>
       </c>
@@ -17700,7 +17755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="263" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C263" s="6">
         <v>-15</v>
       </c>
@@ -17774,7 +17829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="264" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C264" s="6">
         <v>-15</v>
       </c>
@@ -17848,26 +17903,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="265" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C265" s="6"/>
       <c r="D265" s="8"/>
-      <c r="E265" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F265" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G265" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H265" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I265" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J265" s="6" t="b">
-        <v>0</v>
+      <c r="E265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I265" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J265" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K265" s="6" t="b">
         <v>0</v>
@@ -17918,7 +17973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="266" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C266" s="6">
         <v>15</v>
       </c>
@@ -17990,7 +18045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="267" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C267" s="6"/>
       <c r="D267" s="8">
         <v>15</v>
@@ -18062,7 +18117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="268" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C268" s="6">
         <v>15</v>
       </c>
@@ -18136,7 +18191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="269" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C269" s="6">
         <v>-3</v>
       </c>
@@ -18210,7 +18265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C273" s="10" t="s">
         <v>594</v>
       </c>
@@ -18240,7 +18295,7 @@
       <c r="Y273" s="6"/>
       <c r="Z273" s="6"/>
     </row>
-    <row r="274" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="274" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C274" s="6" t="s">
         <v>53</v>
       </c>
@@ -18314,7 +18369,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="275" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C275" s="6" t="s">
         <v>55</v>
       </c>
@@ -18388,7 +18443,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="276" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C276" s="7">
         <v>1</v>
       </c>
@@ -18462,7 +18517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C277" s="7">
         <v>-1</v>
       </c>
@@ -18536,7 +18591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C278" s="6">
         <v>0</v>
       </c>
@@ -18610,7 +18665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C279" s="6">
         <v>-15</v>
       </c>
@@ -18684,7 +18739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C280" s="6">
         <v>-15</v>
       </c>
@@ -18758,26 +18813,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C281" s="6"/>
       <c r="D281" s="8"/>
-      <c r="E281" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F281" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G281" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H281" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I281" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J281" s="6" t="b">
-        <v>0</v>
+      <c r="E281" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F281" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G281" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H281" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I281" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J281" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K281" s="6" t="b">
         <v>0</v>
@@ -18828,7 +18883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C282" s="6">
         <v>15</v>
       </c>
@@ -18900,7 +18955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C283" s="6"/>
       <c r="D283" s="8">
         <v>15</v>
@@ -18972,7 +19027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C284" s="6">
         <v>15</v>
       </c>
@@ -19046,7 +19101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C285" s="6">
         <v>-3</v>
       </c>
@@ -19120,7 +19175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C289" s="10" t="s">
         <v>595</v>
       </c>
@@ -19150,7 +19205,7 @@
       <c r="Y289" s="6"/>
       <c r="Z289" s="6"/>
     </row>
-    <row r="290" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C290" s="6" t="s">
         <v>53</v>
       </c>
@@ -19224,7 +19279,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="291" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C291" s="6" t="s">
         <v>55</v>
       </c>
@@ -19298,7 +19353,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="292" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C292" s="7">
         <v>1</v>
       </c>
@@ -19372,7 +19427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C293" s="7">
         <v>-1</v>
       </c>
@@ -19446,7 +19501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C294" s="6">
         <v>0</v>
       </c>
@@ -19520,7 +19575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C295" s="6">
         <v>-15</v>
       </c>
@@ -19594,7 +19649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C296" s="6">
         <v>-15</v>
       </c>
@@ -19668,26 +19723,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C297" s="6"/>
       <c r="D297" s="8"/>
-      <c r="E297" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F297" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G297" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H297" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I297" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J297" s="6" t="b">
-        <v>0</v>
+      <c r="E297" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F297" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G297" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H297" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I297" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J297" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K297" s="6" t="b">
         <v>0</v>
@@ -19738,7 +19793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C298" s="6">
         <v>15</v>
       </c>
@@ -19810,7 +19865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C299" s="6"/>
       <c r="D299" s="8">
         <v>15</v>
@@ -19882,7 +19937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C300" s="6">
         <v>15</v>
       </c>
@@ -19956,7 +20011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C301" s="6">
         <v>-3</v>
       </c>
@@ -20030,7 +20085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C305" s="10" t="s">
         <v>596</v>
       </c>
@@ -20060,7 +20115,7 @@
       <c r="Y305" s="6"/>
       <c r="Z305" s="6"/>
     </row>
-    <row r="306" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C306" s="6" t="s">
         <v>53</v>
       </c>
@@ -20134,7 +20189,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="307" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C307" s="6" t="s">
         <v>55</v>
       </c>
@@ -20208,7 +20263,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="308" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C308" s="7">
         <v>1</v>
       </c>
@@ -20282,7 +20337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C309" s="7">
         <v>-1</v>
       </c>
@@ -20356,7 +20411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C310" s="6">
         <v>0</v>
       </c>
@@ -20430,7 +20485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C311" s="6">
         <v>-15</v>
       </c>
@@ -20504,7 +20559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C312" s="6">
         <v>-15</v>
       </c>
@@ -20578,26 +20633,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C313" s="6"/>
       <c r="D313" s="8"/>
-      <c r="E313" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F313" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G313" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H313" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I313" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J313" s="6" t="b">
-        <v>0</v>
+      <c r="E313" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F313" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G313" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H313" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I313" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J313" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K313" s="6" t="b">
         <v>0</v>
@@ -20648,7 +20703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C314" s="6">
         <v>15</v>
       </c>
@@ -20720,7 +20775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C315" s="6"/>
       <c r="D315" s="8">
         <v>15</v>
@@ -20792,7 +20847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C316" s="6">
         <v>15</v>
       </c>
@@ -20866,7 +20921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C317" s="6">
         <v>-3</v>
       </c>
@@ -20940,7 +20995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C321" s="10" t="s">
         <v>597</v>
       </c>
@@ -20970,7 +21025,7 @@
       <c r="Y321" s="6"/>
       <c r="Z321" s="6"/>
     </row>
-    <row r="322" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C322" s="6" t="s">
         <v>53</v>
       </c>
@@ -21044,7 +21099,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="323" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C323" s="6" t="s">
         <v>55</v>
       </c>
@@ -21118,7 +21173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="324" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C324" s="7">
         <v>1</v>
       </c>
@@ -21192,7 +21247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C325" s="7">
         <v>-1</v>
       </c>
@@ -21266,7 +21321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C326" s="6">
         <v>0</v>
       </c>
@@ -21340,7 +21395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C327" s="6">
         <v>-15</v>
       </c>
@@ -21414,7 +21469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C328" s="6">
         <v>-15</v>
       </c>
@@ -21488,26 +21543,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C329" s="6"/>
       <c r="D329" s="8"/>
-      <c r="E329" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F329" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G329" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H329" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I329" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J329" s="6" t="b">
-        <v>0</v>
+      <c r="E329" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F329" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G329" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H329" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I329" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J329" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K329" s="6" t="b">
         <v>0</v>
@@ -21558,7 +21613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C330" s="6">
         <v>15</v>
       </c>
@@ -21630,7 +21685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C331" s="6"/>
       <c r="D331" s="8">
         <v>15</v>
@@ -21702,7 +21757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C332" s="6">
         <v>15</v>
       </c>
@@ -21776,7 +21831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C333" s="6">
         <v>-3</v>
       </c>
@@ -21850,7 +21905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C337" s="10" t="s">
         <v>598</v>
       </c>
@@ -21880,7 +21935,7 @@
       <c r="Y337" s="6"/>
       <c r="Z337" s="6"/>
     </row>
-    <row r="338" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C338" s="6" t="s">
         <v>53</v>
       </c>
@@ -21954,7 +22009,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="339" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C339" s="6" t="s">
         <v>55</v>
       </c>
@@ -22028,7 +22083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="340" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C340" s="7">
         <v>1</v>
       </c>
@@ -22102,7 +22157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C341" s="7">
         <v>-1</v>
       </c>
@@ -22176,7 +22231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C342" s="6">
         <v>0</v>
       </c>
@@ -22250,7 +22305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C343" s="6">
         <v>-15</v>
       </c>
@@ -22324,7 +22379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C344" s="6">
         <v>-15</v>
       </c>
@@ -22398,26 +22453,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C345" s="6"/>
       <c r="D345" s="8"/>
-      <c r="E345" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F345" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G345" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H345" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I345" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J345" s="6" t="b">
-        <v>0</v>
+      <c r="E345" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F345" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G345" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H345" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I345" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J345" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K345" s="6" t="b">
         <v>0</v>
@@ -22468,7 +22523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C346" s="6">
         <v>15</v>
       </c>
@@ -22540,7 +22595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C347" s="6"/>
       <c r="D347" s="8">
         <v>15</v>
@@ -22612,7 +22667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C348" s="6">
         <v>15</v>
       </c>
@@ -22686,7 +22741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C349" s="6">
         <v>-3</v>
       </c>
@@ -22760,7 +22815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C353" s="10" t="s">
         <v>599</v>
       </c>
@@ -22790,7 +22845,7 @@
       <c r="Y353" s="6"/>
       <c r="Z353" s="6"/>
     </row>
-    <row r="354" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C354" s="6" t="s">
         <v>53</v>
       </c>
@@ -22864,7 +22919,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="355" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C355" s="6" t="s">
         <v>55</v>
       </c>
@@ -22938,7 +22993,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="356" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C356" s="7">
         <v>1</v>
       </c>
@@ -23012,7 +23067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C357" s="7">
         <v>-1</v>
       </c>
@@ -23086,7 +23141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C358" s="6">
         <v>0</v>
       </c>
@@ -23160,7 +23215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C359" s="6">
         <v>-15</v>
       </c>
@@ -23234,7 +23289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C360" s="6">
         <v>-15</v>
       </c>
@@ -23308,26 +23363,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C361" s="6"/>
       <c r="D361" s="8"/>
-      <c r="E361" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F361" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G361" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H361" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I361" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J361" s="6" t="b">
-        <v>0</v>
+      <c r="E361" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F361" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G361" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H361" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I361" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J361" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K361" s="6" t="b">
         <v>0</v>
@@ -23378,7 +23433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C362" s="6">
         <v>15</v>
       </c>
@@ -23450,7 +23505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C363" s="6"/>
       <c r="D363" s="8">
         <v>15</v>
@@ -23522,7 +23577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C364" s="6">
         <v>15</v>
       </c>
@@ -23596,7 +23651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C365" s="6">
         <v>-3</v>
       </c>
@@ -23670,7 +23725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C369" s="10" t="s">
         <v>600</v>
       </c>
@@ -23700,7 +23755,7 @@
       <c r="Y369" s="6"/>
       <c r="Z369" s="6"/>
     </row>
-    <row r="370" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C370" s="6" t="s">
         <v>53</v>
       </c>
@@ -23774,7 +23829,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="371" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C371" s="6" t="s">
         <v>55</v>
       </c>
@@ -23848,7 +23903,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="372" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C372" s="7">
         <v>1</v>
       </c>
@@ -23922,7 +23977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C373" s="7">
         <v>-1</v>
       </c>
@@ -23996,7 +24051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C374" s="6">
         <v>0</v>
       </c>
@@ -24070,7 +24125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C375" s="6">
         <v>-15</v>
       </c>
@@ -24144,7 +24199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C376" s="6">
         <v>-15</v>
       </c>
@@ -24218,26 +24273,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C377" s="6"/>
       <c r="D377" s="8"/>
-      <c r="E377" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F377" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G377" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H377" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I377" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J377" s="6" t="b">
-        <v>0</v>
+      <c r="E377" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F377" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G377" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H377" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I377" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J377" s="12" t="b">
+        <v>1</v>
       </c>
       <c r="K377" s="6" t="b">
         <v>0</v>
@@ -24288,7 +24343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C378" s="6">
         <v>15</v>
       </c>
@@ -24360,7 +24415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C379" s="6"/>
       <c r="D379" s="8">
         <v>15</v>
@@ -24432,7 +24487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C380" s="6">
         <v>15</v>
       </c>
@@ -24506,7 +24561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C381" s="6">
         <v>-3</v>
       </c>
@@ -24582,12 +24637,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C305:D305"/>
+    <mergeCell ref="C321:D321"/>
+    <mergeCell ref="C337:D337"/>
+    <mergeCell ref="C353:D353"/>
+    <mergeCell ref="C369:D369"/>
     <mergeCell ref="C289:D289"/>
     <mergeCell ref="C113:D113"/>
     <mergeCell ref="C129:D129"/>
@@ -24600,11 +24654,12 @@
     <mergeCell ref="C241:D241"/>
     <mergeCell ref="C257:D257"/>
     <mergeCell ref="C273:D273"/>
-    <mergeCell ref="C305:D305"/>
-    <mergeCell ref="C321:D321"/>
-    <mergeCell ref="C337:D337"/>
-    <mergeCell ref="C353:D353"/>
-    <mergeCell ref="C369:D369"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C81:D81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>